<commit_message>
fixed docstring - Attributes StaticPlotter missing
</commit_message>
<xml_diff>
--- a/sedimentanalyst/analyzer/outputs/global_dataframe.xlsx
+++ b/sedimentanalyst/analyzer/outputs/global_dataframe.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -17,8 +17,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -57,19 +57,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AX5"/>
+  <dimension ref="A1:AX3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -961,315 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>KB07 FC 1 1 Dez2019</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>44330</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6145885.1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1394514.2</v>
-      </c>
-      <c r="F4" t="n">
-        <v>3.002469135802469</v>
-      </c>
-      <c r="G4" t="n">
-        <v>8.166399999999999</v>
-      </c>
-      <c r="H4" t="n">
-        <v>19.97575</v>
-      </c>
-      <c r="I4" t="n">
-        <v>27.2437</v>
-      </c>
-      <c r="J4" t="n">
-        <v>47.53545310015899</v>
-      </c>
-      <c r="K4" t="n">
-        <v>56.92836248012719</v>
-      </c>
-      <c r="L4" t="n">
-        <v>78.78092209856916</v>
-      </c>
-      <c r="M4" t="n">
-        <v>95.41979014308427</v>
-      </c>
-      <c r="N4" t="n">
-        <v>106.5123688394277</v>
-      </c>
-      <c r="O4" t="n">
-        <v>51.52596150276046</v>
-      </c>
-      <c r="P4" t="n">
-        <v>27.91480206314355</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>3.418250644487602</v>
-      </c>
-      <c r="R4" t="n">
-        <v>8.166399999999999</v>
-      </c>
-      <c r="S4" t="n">
-        <v>37.49455976436801</v>
-      </c>
-      <c r="T4" t="n">
-        <v>2.412353408090465</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.6255915086700388</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0.7149842042065249</v>
-      </c>
-      <c r="W4" t="n">
-        <v>18.9605154641871</v>
-      </c>
-      <c r="X4" t="n">
-        <v>4.342351098574596</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.1740375412767036</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0.2233344029409659</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>0.2062080425451858</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.1995931522976197</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>0.1778</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>5.764075195605861e-05</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>0.0001377590643970584</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0.0001038065714690175</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>9.25841743780763e-05</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>6.202428437794134e-05</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>100</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>100</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>66.4640648325869</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>32.92812966517381</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>22.26487523992322</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>15.86692258477287</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>11.29238643634037</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>8.701215611004478</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>7.698869695030924</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>7.28300277244615</v>
-      </c>
-      <c r="AS4" t="n">
-        <v>4.851780763489017</v>
-      </c>
-      <c r="AT4" t="n">
-        <v>1.140968223501813</v>
-      </c>
-      <c r="AU4" t="n">
-        <v>0.3838771593090211</v>
-      </c>
-      <c r="AV4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>MS2_FC1</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>44377</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4585621.74</v>
-      </c>
-      <c r="E5" t="n">
-        <v>5350853.14199999</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.388400900900901</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.9842748091603053</v>
-      </c>
-      <c r="H5" t="n">
-        <v>4.036516853932585</v>
-      </c>
-      <c r="I5" t="n">
-        <v>5.558426966292136</v>
-      </c>
-      <c r="J5" t="n">
-        <v>12.59062776304156</v>
-      </c>
-      <c r="K5" t="n">
-        <v>16.77177352206495</v>
-      </c>
-      <c r="L5" t="n">
-        <v>27.26040799333889</v>
-      </c>
-      <c r="M5" t="n">
-        <v>36.38526315789473</v>
-      </c>
-      <c r="N5" t="n">
-        <v>46.36578947368421</v>
-      </c>
-      <c r="O5" t="n">
-        <v>18.33282586721245</v>
-      </c>
-      <c r="P5" t="n">
-        <v>5.984404561105835</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>6.08001394063025</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.9842748091603053</v>
-      </c>
-      <c r="S5" t="n">
-        <v>20.48516281728311</v>
-      </c>
-      <c r="T5" t="n">
-        <v>2.41928361563929</v>
-      </c>
-      <c r="U5" t="n">
-        <v>4.114260507539901</v>
-      </c>
-      <c r="V5" t="n">
-        <v>39.1627205959093</v>
-      </c>
-      <c r="W5" t="n">
-        <v>43.18160303738379</v>
-      </c>
-      <c r="X5" t="n">
-        <v>4.742906788039636</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.2407575035744048</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0.2533658223034426</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0.2055559931530012</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.2084296517518845</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>7.266105503195829e-05</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>8.756924013584426e-05</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>4.130352012745834e-05</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>4.337332295245306e-05</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>3.751744332107799e-05</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>100</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>100</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>100</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>81.06312292358804</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>58.89627168696936</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>38.02141011443337</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>24.88002953119232</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>18.82613510520487</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>16.07604282022887</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>13.65817644887412</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>5.46327057954965</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>1.144333702473237</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>0.4983388704318937</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>